<commit_message>
fix: some improvement in input masal
</commit_message>
<xml_diff>
--- a/public/export.xlsx
+++ b/public/export.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>Nama Lengkap</t>
   </si>
@@ -38,82 +38,16 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Ucok Baba</t>
-  </si>
-  <si>
-    <t>10ucokbaba@gmail.com</t>
-  </si>
-  <si>
-    <t>SMK 2 Medan</t>
+    <t xml:space="preserve">Andrian Putra </t>
+  </si>
+  <si>
+    <t>ramadanand89@gmail.com</t>
   </si>
   <si>
     <t>VII - A</t>
   </si>
   <si>
-    <t>odit</t>
-  </si>
-  <si>
-    <t>maxime</t>
-  </si>
-  <si>
-    <t>Ucok mnimal</t>
-  </si>
-  <si>
-    <t>3ucokbaba2@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMK 2 Medan </t>
-  </si>
-  <si>
-    <t>voluptates</t>
-  </si>
-  <si>
-    <t>repellat</t>
-  </si>
-  <si>
-    <t>fdasfsdaf</t>
-  </si>
-  <si>
-    <t>323232@gmail.com</t>
-  </si>
-  <si>
-    <t>dfdf</t>
-  </si>
-  <si>
-    <t>et</t>
-  </si>
-  <si>
-    <t>dolore</t>
-  </si>
-  <si>
-    <t>dfasfsda</t>
-  </si>
-  <si>
-    <t>5dfdfdfd@gmail.com</t>
-  </si>
-  <si>
-    <t>VII - B</t>
-  </si>
-  <si>
-    <t>molestias</t>
-  </si>
-  <si>
-    <t>dolores</t>
-  </si>
-  <si>
-    <t>asdfasfa</t>
-  </si>
-  <si>
-    <t>6dfdfdf@gmail.com</t>
-  </si>
-  <si>
-    <t>VII - C</t>
-  </si>
-  <si>
-    <t>culpa</t>
-  </si>
-  <si>
-    <t>atque</t>
+    <t>eItFafz5lj</t>
   </si>
 </sst>
 </file>
@@ -453,7 +387,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,114 +423,22 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>545565</v>
+        <v>21212344</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>3232</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4">
-        <v>55553</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5">
-        <v>33455343</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6">
-        <v>34455</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" t="s">
-        <v>32</v>
+      <c r="G2">
+        <v>12345678</v>
       </c>
     </row>
   </sheetData>

</xml_diff>